<commit_message>
del 1 word; use iframe
</commit_message>
<xml_diff>
--- a/source/assets/SampleWordList.xlsx
+++ b/source/assets/SampleWordList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="运算符" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="150">
   <si>
     <t xml:space="preserve">语法类型</t>
   </si>
@@ -172,164 +172,155 @@
     <t xml:space="preserve">输出默认标记</t>
   </si>
   <si>
+    <t xml:space="preserve">模板 → 模板</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temporal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">进行态</t>
+  </si>
+  <si>
+    <t xml:space="preserve">完成态</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">大小</t>
+  </si>
+  <si>
     <t xml:space="preserve">运算符 → 模板</t>
   </si>
   <si>
+    <t xml:space="preserve">OrdinalNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">序数</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">值</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inverse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">右逆</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GraphProperty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">析取结构</t>
+  </si>
+  <si>
+    <t xml:space="preserve">合取结构</t>
+  </si>
+  <si>
+    <t xml:space="preserve">连通性</t>
+  </si>
+  <si>
+    <t xml:space="preserve">跟随输入</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LA</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">因果（使动</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">被动）</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">假想（意动）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">需求（应当）</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">符号式</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">^n → </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">模板</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">短普通模板</t>
+  </si>
+  <si>
+    <t xml:space="preserve">无限制</t>
+  </si>
+  <si>
     <t xml:space="preserve">Logic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Meta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">存在性</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LI: forall f (LI[KO[f]][x] &lt;=&gt; exist y f[y,x])</t>
-  </si>
-  <si>
-    <t xml:space="preserve">模板 → 模板</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temporal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State</t>
-  </si>
-  <si>
-    <t xml:space="preserve">进行态</t>
-  </si>
-  <si>
-    <t xml:space="preserve">完成态</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Order</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Relation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">大小</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OrdinalNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">序数</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Result</t>
-  </si>
-  <si>
-    <t xml:space="preserve">值</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inverse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">右逆</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GraphProperty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">析取结构</t>
-  </si>
-  <si>
-    <t xml:space="preserve">合取结构</t>
-  </si>
-  <si>
-    <t xml:space="preserve">连通性</t>
-  </si>
-  <si>
-    <t xml:space="preserve">跟随输入</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LA</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">因果（使动</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">被动）</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">ta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">假想（意动）</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">需求（应当）</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">符号式</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">^n → </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">模板</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">短普通模板</t>
-  </si>
-  <si>
-    <t xml:space="preserve">无限制</t>
   </si>
   <si>
     <t xml:space="preserve">Formal</t>
@@ -984,16 +975,12 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1026,7 +1013,7 @@
   </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1138,7 +1125,7 @@
       <c r="E5" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="0" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="0" t="s">
@@ -1178,10 +1165,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1250,65 +1237,62 @@
       <c r="C2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1316,33 +1300,33 @@
         <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="0" t="s">
         <v>45</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1350,115 +1334,98 @@
         <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="0" t="s">
         <v>50</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>54</v>
+        <v>48</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>55</v>
+      <c r="L10" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" s="0" t="s">
+      <c r="E11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K11" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="L11" s="0" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>60</v>
+      <c r="F12" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>63</v>
+      <c r="E13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1480,7 +1447,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1531,10 +1498,10 @@
     </row>
     <row r="2" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>11</v>
@@ -1549,383 +1516,383 @@
         <v>9</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="F3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="H3" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="I3" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>72</v>
       </c>
       <c r="J3" s="0" t="s">
         <v>15</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="J4" s="0" t="s">
         <v>15</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F9" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="F11" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="G14" s="0" t="s">
         <v>106</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="F18" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="G18" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1985,7 +1952,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I1" s="0" t="s">
         <v>1</v>
@@ -2005,10 +1972,10 @@
     </row>
     <row r="2" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>11</v>
@@ -2016,44 +1983,44 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="I3" s="0" t="s">
         <v>8</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F13" s="4"/>
+      <c r="F13" s="3"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D51" s="4"/>
+      <c r="D51" s="3"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D52" s="4"/>
+      <c r="D52" s="3"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D53" s="4"/>
+      <c r="D53" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2086,13 +2053,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>26</v>
@@ -2100,73 +2067,73 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>15</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>